<commit_message>
weights added in Returns Data.xlsx file
</commit_message>
<xml_diff>
--- a/Returns Data.xlsx
+++ b/Returns Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chait\OneDrive\Desktop\GaTech Studies\Spring 2021\Derivatives\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chait\OneDrive\Desktop\GaTech Studies\Spring 2021\Derivatives\Final Project\derivative-securities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92409E7F-ACE6-4A62-8FC2-FF7C97603434}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A646373-5071-4D5E-A0B5-F779BEBA9AE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22670" yWindow="-2890" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,28 +98,28 @@
     <t>$</t>
   </si>
   <si>
-    <t>Portfolio Return</t>
-  </si>
-  <si>
-    <t>Portfolio variance</t>
-  </si>
-  <si>
-    <t>Portfolio Volatility</t>
-  </si>
-  <si>
     <t>Portfolio Sharpe</t>
   </si>
   <si>
     <t>Portfolio Ret</t>
   </si>
   <si>
-    <t>Variance (10 year)</t>
+    <t>Portfolio Return (Annual)</t>
   </si>
   <si>
-    <t>Returns (10 year)</t>
+    <t>Returns (Annual)</t>
   </si>
   <si>
-    <t>Volatility (10 year)</t>
+    <t>Variance (Annual)</t>
+  </si>
+  <si>
+    <t>Volatility (Annual)</t>
+  </si>
+  <si>
+    <t>Portfolio Variance (Annual)</t>
+  </si>
+  <si>
+    <t>Portfolio Volatility (Annual)</t>
   </si>
 </sst>
 </file>
@@ -129,7 +129,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$$-409]#,##0"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -224,7 +224,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -518,7 +518,7 @@
   <dimension ref="A1:Q2516"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +528,7 @@
     <col min="3" max="4" width="8.7109375" style="3"/>
     <col min="6" max="6" width="8.7109375" style="2"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -551,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -640,31 +640,31 @@
         <v>2.0168039175660506E-2</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J3" s="6">
-        <f>AVERAGE(A2:A2516)*10*252</f>
-        <v>2.4282384811216144</v>
+        <f>AVERAGE(A2:A2516)*252</f>
+        <v>0.24282384811216146</v>
       </c>
       <c r="K3" s="6">
-        <f t="shared" ref="K3:O3" si="2">AVERAGE(B2:B2516)*10*252</f>
-        <v>1.452994573827548</v>
+        <f t="shared" ref="K3:O3" si="2">AVERAGE(B2:B2516)*252</f>
+        <v>0.14529945738275482</v>
       </c>
       <c r="L3" s="6">
         <f t="shared" si="2"/>
-        <v>0.9814652125392207</v>
+        <v>9.8146521253922078E-2</v>
       </c>
       <c r="M3" s="6">
         <f t="shared" si="2"/>
-        <v>4.9591800125866374</v>
+        <v>0.49591800125866375</v>
       </c>
       <c r="N3" s="6">
         <f t="shared" si="2"/>
-        <v>0.36998152354232328</v>
+        <v>3.699815235423233E-2</v>
       </c>
       <c r="O3" s="6">
         <f t="shared" si="2"/>
-        <v>1.6298927684597957</v>
+        <v>0.16298927684597958</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -693,31 +693,31 @@
         <v>6.1373650867109861E-3</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" s="6">
-        <f>_xlfn.VAR.P(A2:A2516)*10*252</f>
-        <v>0.81935552673123113</v>
+        <f>_xlfn.VAR.P(A2:A2516)*252</f>
+        <v>8.1935552673123122E-2</v>
       </c>
       <c r="K4" s="6">
-        <f t="shared" ref="K4:O4" si="3">_xlfn.VAR.P(B2:B2516)*10*252</f>
-        <v>0.83006362569145975</v>
+        <f t="shared" ref="K4:O4" si="3">_xlfn.VAR.P(B2:B2516)*252</f>
+        <v>8.3006362569145967E-2</v>
       </c>
       <c r="L4" s="6">
         <f t="shared" si="3"/>
-        <v>0.41567085073625254</v>
+        <v>4.1567085073625255E-2</v>
       </c>
       <c r="M4" s="6">
         <f t="shared" si="3"/>
-        <v>3.0501368951652061</v>
+        <v>0.30501368951652064</v>
       </c>
       <c r="N4" s="6">
         <f t="shared" si="3"/>
-        <v>0.79563000078368706</v>
+        <v>7.9563000078368709E-2</v>
       </c>
       <c r="O4" s="6">
         <f t="shared" si="3"/>
-        <v>1.6961754354065071</v>
+        <v>0.1696175435406507</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -746,31 +746,31 @@
         <v>-6.5858088295043899E-3</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J5" s="6">
         <f>SQRT(J4)</f>
-        <v>0.90518259303371007</v>
+        <v>0.28624386923237871</v>
       </c>
       <c r="K5" s="6">
         <f t="shared" ref="K5:O5" si="4">SQRT(K4)</f>
-        <v>0.91107827637994954</v>
+        <v>0.28810824800610269</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="4"/>
-        <v>0.64472540723648586</v>
+        <v>0.20388007522469001</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" si="4"/>
-        <v>1.7464641121893132</v>
+        <v>0.55228044462620673</v>
       </c>
       <c r="N5" s="6">
         <f t="shared" si="4"/>
-        <v>0.89198094193972943</v>
+        <v>0.28206914059919547</v>
       </c>
       <c r="O5" s="6">
         <f t="shared" si="4"/>
-        <v>1.3023730016421973</v>
+        <v>0.41184650482995566</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -803,27 +803,27 @@
       </c>
       <c r="J6" s="8">
         <f>(J3-0)/J5</f>
-        <v>2.6825952021275601</v>
+        <v>0.84831108789628618</v>
       </c>
       <c r="K6" s="8">
         <f t="shared" ref="K6:O6" si="5">(K3-0)/K5</f>
-        <v>1.5948076158733935</v>
+        <v>0.50432244959428274</v>
       </c>
       <c r="L6" s="8">
         <f t="shared" si="5"/>
-        <v>1.5222995736217642</v>
+        <v>0.48139339337479542</v>
       </c>
       <c r="M6" s="8">
         <f t="shared" si="5"/>
-        <v>2.8395544906845887</v>
+        <v>0.89794597307226753</v>
       </c>
       <c r="N6" s="8">
         <f t="shared" si="5"/>
-        <v>0.41478635489425364</v>
+        <v>0.13116696238247716</v>
       </c>
       <c r="O6" s="8">
         <f t="shared" si="5"/>
-        <v>1.2514792355220969</v>
+        <v>0.39575248286561288</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -957,11 +957,11 @@
         <v>9.3861101985605322E-3</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J9" s="11">
         <f>SUMPRODUCT(J7:O7,J3:O3)</f>
-        <v>2.9248622783976335</v>
+        <v>0.29248622783976341</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -995,11 +995,11 @@
         <v>-5.8401772598074709E-3</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J10" s="6">
-        <f>_xlfn.VAR.P(G2:G2516)*10*252</f>
-        <v>0.72907260309824573</v>
+        <f>_xlfn.VAR.P(G2:G2516)*252</f>
+        <v>7.290726030982457E-2</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1033,11 +1033,11 @@
         <v>-1.6480535952479679E-2</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J11" s="11">
         <f>SQRT(J10)</f>
-        <v>0.85385748406759643</v>
+        <v>0.27001344468345378</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1071,11 +1071,11 @@
         <v>-2.9509337763250532E-2</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J12" s="2">
         <f>J9/J11</f>
-        <v>3.4254689254045165</v>
+        <v>1.083228385840769</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>

</xml_diff>